<commit_message>
Added: today indicator and month selector
</commit_message>
<xml_diff>
--- a/mymonth/static/initial_data/import_me.xlsx
+++ b/mymonth/static/initial_data/import_me.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plr03474\NoOneDrive\Python\myMonth\mymonth\static\initial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D0854A-5D58-4C9B-8FC2-B64693AE84C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBD1478-4B54-476D-822B-B8A845F70F95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16650" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2325" yWindow="-13575" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>id</t>
   </si>
@@ -106,7 +106,16 @@
     <t>24m</t>
   </si>
   <si>
-    <t>2h21m</t>
+    <t>2h 27m</t>
+  </si>
+  <si>
+    <t>1h 3m</t>
+  </si>
+  <si>
+    <t>1h 56m</t>
+  </si>
+  <si>
+    <t>1h 19m</t>
   </si>
 </sst>
 </file>
@@ -114,7 +123,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -170,7 +179,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,8 +485,8 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,26 +684,44 @@
       <c r="A13" s="2">
         <v>44239</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>28</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
+      </c>
+      <c r="H13">
+        <v>7.8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44240</v>
       </c>
+      <c r="H14">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44241</v>
       </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44242</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>